<commit_message>
Created test algoritm Poisson distributions
</commit_message>
<xml_diff>
--- a/Intermediate_data/max_min_poisson.xlsx
+++ b/Intermediate_data/max_min_poisson.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Min count consumer</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>P_min_poisson</t>
+          <t>P_min_poisson_kW</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>P_max_poisson</t>
+          <t>Max count consumer</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>P_max_poisson_kW</t>
         </is>
       </c>
     </row>
@@ -459,2754 +464,3185 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>0:00</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>267</v>
+      </c>
       <c r="D2" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E2" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F2" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>0:10</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>267</v>
+      </c>
       <c r="D3" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E3" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F3" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>0:20</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>267</v>
+      </c>
       <c r="D4" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E4" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F4" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>0:30</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>267</v>
+      </c>
       <c r="D5" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E5" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F5" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>40</v>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>0:40</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>267</v>
+      </c>
       <c r="D6" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E6" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F6" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>50</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>0:50</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>267</v>
+      </c>
       <c r="D7" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E7" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F7" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>60</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>1:00</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D8" t="n">
-        <v>65.47199999999999</v>
+        <v>66.21599999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>82.336</v>
+        <v>347</v>
+      </c>
+      <c r="F8" t="n">
+        <v>86.056</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
-        <v>70</v>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>1:10</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D9" t="n">
-        <v>65.47199999999999</v>
+        <v>66.21599999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>82.336</v>
+        <v>347</v>
+      </c>
+      <c r="F9" t="n">
+        <v>86.056</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>80</v>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>1:20</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D10" t="n">
-        <v>65.47199999999999</v>
+        <v>66.21599999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>82.336</v>
+        <v>347</v>
+      </c>
+      <c r="F10" t="n">
+        <v>86.056</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>90</v>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>1:30</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D11" t="n">
-        <v>65.47199999999999</v>
+        <v>66.21599999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>82.336</v>
+        <v>347</v>
+      </c>
+      <c r="F11" t="n">
+        <v>86.056</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
-        <v>100</v>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>1:40</t>
         </is>
       </c>
+      <c r="C12" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D12" t="n">
-        <v>65.47199999999999</v>
+        <v>66.21599999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>82.336</v>
+        <v>347</v>
+      </c>
+      <c r="F12" t="n">
+        <v>86.056</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
-        <v>110</v>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>1:50</t>
         </is>
       </c>
+      <c r="C13" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D13" t="n">
-        <v>65.47199999999999</v>
+        <v>66.21599999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>82.336</v>
+        <v>347</v>
+      </c>
+      <c r="F13" t="n">
+        <v>86.056</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="n">
-        <v>120</v>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>2:00</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>267</v>
+      </c>
       <c r="D14" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E14" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F14" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="n">
-        <v>130</v>
-      </c>
-      <c r="C15" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>2:10</t>
         </is>
       </c>
+      <c r="C15" t="n">
+        <v>267</v>
+      </c>
       <c r="D15" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E15" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F15" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="n">
-        <v>140</v>
-      </c>
-      <c r="C16" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>2:20</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>267</v>
+      </c>
       <c r="D16" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E16" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F16" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
-        <v>150</v>
-      </c>
-      <c r="C17" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>2:30</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>267</v>
+      </c>
       <c r="D17" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E17" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F17" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="n">
-        <v>160</v>
-      </c>
-      <c r="C18" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>2:40</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>267</v>
+      </c>
       <c r="D18" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E18" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F18" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="n">
-        <v>170</v>
-      </c>
-      <c r="C19" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>2:50</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>267</v>
+      </c>
       <c r="D19" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E19" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F19" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="n">
-        <v>180</v>
-      </c>
-      <c r="C20" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>3:00</t>
         </is>
       </c>
+      <c r="C20" t="n">
+        <v>267</v>
+      </c>
       <c r="D20" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E20" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F20" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="n">
-        <v>190</v>
-      </c>
-      <c r="C21" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>3:10</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>267</v>
+      </c>
       <c r="D21" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E21" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F21" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="n">
-        <v>200</v>
-      </c>
-      <c r="C22" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>3:20</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>267</v>
+      </c>
       <c r="D22" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E22" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F22" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="n">
-        <v>210</v>
-      </c>
-      <c r="C23" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>3:30</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>267</v>
+      </c>
       <c r="D23" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E23" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F23" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="n">
-        <v>220</v>
-      </c>
-      <c r="C24" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>3:40</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>267</v>
+      </c>
       <c r="D24" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E24" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F24" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="n">
-        <v>230</v>
-      </c>
-      <c r="C25" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>3:50</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>267</v>
+      </c>
       <c r="D25" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E25" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F25" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="n">
-        <v>240</v>
-      </c>
-      <c r="C26" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>4:00</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>267</v>
+      </c>
       <c r="D26" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E26" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F26" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="n">
-        <v>250</v>
-      </c>
-      <c r="C27" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>4:10</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>267</v>
+      </c>
       <c r="D27" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E27" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F27" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="n">
-        <v>260</v>
-      </c>
-      <c r="C28" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>4:20</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>267</v>
+      </c>
       <c r="D28" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E28" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F28" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="n">
-        <v>270</v>
-      </c>
-      <c r="C29" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>4:30</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>267</v>
+      </c>
       <c r="D29" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E29" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F29" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="n">
-        <v>280</v>
-      </c>
-      <c r="C30" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>4:40</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>267</v>
+      </c>
       <c r="D30" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E30" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F30" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="n">
-        <v>290</v>
-      </c>
-      <c r="C31" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>4:50</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>267</v>
+      </c>
       <c r="D31" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E31" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F31" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="n">
-        <v>300</v>
-      </c>
-      <c r="C32" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>5:00</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>267</v>
+      </c>
       <c r="D32" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E32" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F32" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="n">
-        <v>310</v>
-      </c>
-      <c r="C33" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>5:10</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>267</v>
+      </c>
       <c r="D33" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E33" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F33" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="n">
-        <v>320</v>
-      </c>
-      <c r="C34" t="inlineStr">
+      <c r="B34" t="inlineStr">
         <is>
           <t>5:20</t>
         </is>
       </c>
+      <c r="C34" t="n">
+        <v>267</v>
+      </c>
       <c r="D34" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E34" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F34" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="n">
-        <v>330</v>
-      </c>
-      <c r="C35" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>5:30</t>
         </is>
       </c>
+      <c r="C35" t="n">
+        <v>267</v>
+      </c>
       <c r="D35" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E35" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F35" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="n">
-        <v>340</v>
-      </c>
-      <c r="C36" t="inlineStr">
+      <c r="B36" t="inlineStr">
         <is>
           <t>5:40</t>
         </is>
       </c>
+      <c r="C36" t="n">
+        <v>267</v>
+      </c>
       <c r="D36" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E36" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F36" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="n">
-        <v>350</v>
-      </c>
-      <c r="C37" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>5:50</t>
         </is>
       </c>
+      <c r="C37" t="n">
+        <v>267</v>
+      </c>
       <c r="D37" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E37" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F37" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="n">
-        <v>360</v>
-      </c>
-      <c r="C38" t="inlineStr">
+      <c r="B38" t="inlineStr">
         <is>
           <t>6:00</t>
         </is>
       </c>
+      <c r="C38" t="n">
+        <v>267</v>
+      </c>
       <c r="D38" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E38" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F38" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="n">
-        <v>370</v>
-      </c>
-      <c r="C39" t="inlineStr">
+      <c r="B39" t="inlineStr">
         <is>
           <t>6:10</t>
         </is>
       </c>
+      <c r="C39" t="n">
+        <v>267</v>
+      </c>
       <c r="D39" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E39" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F39" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="n">
-        <v>380</v>
-      </c>
-      <c r="C40" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>6:20</t>
         </is>
       </c>
+      <c r="C40" t="n">
+        <v>267</v>
+      </c>
       <c r="D40" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E40" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F40" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="n">
-        <v>390</v>
-      </c>
-      <c r="C41" t="inlineStr">
+      <c r="B41" t="inlineStr">
         <is>
           <t>6:30</t>
         </is>
       </c>
+      <c r="C41" t="n">
+        <v>267</v>
+      </c>
       <c r="D41" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E41" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F41" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="n">
-        <v>400</v>
-      </c>
-      <c r="C42" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>6:40</t>
         </is>
       </c>
+      <c r="C42" t="n">
+        <v>267</v>
+      </c>
       <c r="D42" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E42" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F42" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="n">
-        <v>410</v>
-      </c>
-      <c r="C43" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>6:50</t>
         </is>
       </c>
+      <c r="C43" t="n">
+        <v>267</v>
+      </c>
       <c r="D43" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E43" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F43" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="n">
-        <v>420</v>
-      </c>
-      <c r="C44" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>7:00</t>
         </is>
       </c>
+      <c r="C44" t="n">
+        <v>267</v>
+      </c>
       <c r="D44" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E44" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F44" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="n">
-        <v>430</v>
-      </c>
-      <c r="C45" t="inlineStr">
+      <c r="B45" t="inlineStr">
         <is>
           <t>7:10</t>
         </is>
       </c>
+      <c r="C45" t="n">
+        <v>267</v>
+      </c>
       <c r="D45" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E45" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F45" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="n">
-        <v>440</v>
-      </c>
-      <c r="C46" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>7:20</t>
         </is>
       </c>
+      <c r="C46" t="n">
+        <v>267</v>
+      </c>
       <c r="D46" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E46" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F46" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="n">
-        <v>450</v>
-      </c>
-      <c r="C47" t="inlineStr">
+      <c r="B47" t="inlineStr">
         <is>
           <t>7:30</t>
         </is>
       </c>
+      <c r="C47" t="n">
+        <v>267</v>
+      </c>
       <c r="D47" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E47" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F47" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="n">
-        <v>460</v>
-      </c>
-      <c r="C48" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>7:40</t>
         </is>
       </c>
+      <c r="C48" t="n">
+        <v>267</v>
+      </c>
       <c r="D48" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E48" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F48" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="n">
-        <v>470</v>
-      </c>
-      <c r="C49" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>7:50</t>
         </is>
       </c>
+      <c r="C49" t="n">
+        <v>267</v>
+      </c>
       <c r="D49" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E49" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F49" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="n">
-        <v>480</v>
-      </c>
-      <c r="C50" t="inlineStr">
+      <c r="B50" t="inlineStr">
         <is>
           <t>8:00</t>
         </is>
       </c>
+      <c r="C50" t="n">
+        <v>267</v>
+      </c>
       <c r="D50" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E50" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F50" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="n">
-        <v>490</v>
-      </c>
-      <c r="C51" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>8:10</t>
         </is>
       </c>
+      <c r="C51" t="n">
+        <v>267</v>
+      </c>
       <c r="D51" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E51" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F51" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="n">
-        <v>500</v>
-      </c>
-      <c r="C52" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>8:20</t>
         </is>
       </c>
+      <c r="C52" t="n">
+        <v>267</v>
+      </c>
       <c r="D52" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E52" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F52" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="n">
-        <v>510</v>
-      </c>
-      <c r="C53" t="inlineStr">
+      <c r="B53" t="inlineStr">
         <is>
           <t>8:30</t>
         </is>
       </c>
+      <c r="C53" t="n">
+        <v>267</v>
+      </c>
       <c r="D53" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E53" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F53" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="n">
-        <v>520</v>
-      </c>
-      <c r="C54" t="inlineStr">
+      <c r="B54" t="inlineStr">
         <is>
           <t>8:40</t>
         </is>
       </c>
+      <c r="C54" t="n">
+        <v>267</v>
+      </c>
       <c r="D54" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E54" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F54" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="n">
-        <v>530</v>
-      </c>
-      <c r="C55" t="inlineStr">
+      <c r="B55" t="inlineStr">
         <is>
           <t>8:50</t>
         </is>
       </c>
+      <c r="C55" t="n">
+        <v>267</v>
+      </c>
       <c r="D55" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E55" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F55" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="n">
-        <v>540</v>
-      </c>
-      <c r="C56" t="inlineStr">
+      <c r="B56" t="inlineStr">
         <is>
           <t>9:00</t>
         </is>
       </c>
+      <c r="C56" t="n">
+        <v>267</v>
+      </c>
       <c r="D56" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E56" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F56" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="n">
-        <v>550</v>
-      </c>
-      <c r="C57" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>9:10</t>
         </is>
       </c>
+      <c r="C57" t="n">
+        <v>267</v>
+      </c>
       <c r="D57" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E57" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F57" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="n">
-        <v>560</v>
-      </c>
-      <c r="C58" t="inlineStr">
+      <c r="B58" t="inlineStr">
         <is>
           <t>9:20</t>
         </is>
       </c>
+      <c r="C58" t="n">
+        <v>267</v>
+      </c>
       <c r="D58" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E58" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F58" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="n">
-        <v>570</v>
-      </c>
-      <c r="C59" t="inlineStr">
+      <c r="B59" t="inlineStr">
         <is>
           <t>9:30</t>
         </is>
       </c>
+      <c r="C59" t="n">
+        <v>267</v>
+      </c>
       <c r="D59" t="n">
-        <v>696.432</v>
+        <v>704.346</v>
       </c>
       <c r="E59" t="n">
-        <v>875.816</v>
+        <v>347</v>
+      </c>
+      <c r="F59" t="n">
+        <v>915.386</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="n">
-        <v>580</v>
-      </c>
-      <c r="C60" t="inlineStr">
+      <c r="B60" t="inlineStr">
         <is>
           <t>9:40</t>
         </is>
       </c>
+      <c r="C60" t="n">
+        <v>267</v>
+      </c>
       <c r="D60" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E60" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F60" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B61" t="n">
-        <v>590</v>
-      </c>
-      <c r="C61" t="inlineStr">
+      <c r="B61" t="inlineStr">
         <is>
           <t>9:50</t>
         </is>
       </c>
+      <c r="C61" t="n">
+        <v>267</v>
+      </c>
       <c r="D61" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E61" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F61" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="n">
-        <v>600</v>
-      </c>
-      <c r="C62" t="inlineStr">
+      <c r="B62" t="inlineStr">
         <is>
           <t>10:00</t>
         </is>
       </c>
+      <c r="C62" t="n">
+        <v>267</v>
+      </c>
       <c r="D62" t="n">
-        <v>1963.632</v>
+        <v>1985.946</v>
       </c>
       <c r="E62" t="n">
-        <v>2469.416</v>
+        <v>347</v>
+      </c>
+      <c r="F62" t="n">
+        <v>2580.986</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="n">
-        <v>610</v>
-      </c>
-      <c r="C63" t="inlineStr">
+      <c r="B63" t="inlineStr">
         <is>
           <t>10:10</t>
         </is>
       </c>
+      <c r="C63" t="n">
+        <v>267</v>
+      </c>
       <c r="D63" t="n">
-        <v>1963.632</v>
+        <v>1985.946</v>
       </c>
       <c r="E63" t="n">
-        <v>2469.416</v>
+        <v>347</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2580.986</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="n">
-        <v>620</v>
-      </c>
-      <c r="C64" t="inlineStr">
+      <c r="B64" t="inlineStr">
         <is>
           <t>10:20</t>
         </is>
       </c>
+      <c r="C64" t="n">
+        <v>267</v>
+      </c>
       <c r="D64" t="n">
-        <v>1966.272</v>
+        <v>1988.616</v>
       </c>
       <c r="E64" t="n">
-        <v>2472.736</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F64" t="n">
+        <v>2584.456</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="n">
-        <v>630</v>
-      </c>
-      <c r="C65" t="inlineStr">
+      <c r="B65" t="inlineStr">
         <is>
           <t>10:30</t>
         </is>
       </c>
+      <c r="C65" t="n">
+        <v>267</v>
+      </c>
       <c r="D65" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E65" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F65" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B66" t="n">
-        <v>640</v>
-      </c>
-      <c r="C66" t="inlineStr">
+      <c r="B66" t="inlineStr">
         <is>
           <t>10:40</t>
         </is>
       </c>
+      <c r="C66" t="n">
+        <v>267</v>
+      </c>
       <c r="D66" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E66" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F66" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67" t="n">
-        <v>650</v>
-      </c>
-      <c r="C67" t="inlineStr">
+      <c r="B67" t="inlineStr">
         <is>
           <t>10:50</t>
         </is>
       </c>
+      <c r="C67" t="n">
+        <v>267</v>
+      </c>
       <c r="D67" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E67" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F67" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="n">
-        <v>660</v>
-      </c>
-      <c r="C68" t="inlineStr">
+      <c r="B68" t="inlineStr">
         <is>
           <t>11:00</t>
         </is>
       </c>
+      <c r="C68" t="n">
+        <v>267</v>
+      </c>
       <c r="D68" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E68" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F68" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69" t="n">
-        <v>670</v>
-      </c>
-      <c r="C69" t="inlineStr">
+      <c r="B69" t="inlineStr">
         <is>
           <t>11:10</t>
         </is>
       </c>
+      <c r="C69" t="n">
+        <v>267</v>
+      </c>
       <c r="D69" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E69" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F69" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70" t="n">
-        <v>680</v>
-      </c>
-      <c r="C70" t="inlineStr">
+      <c r="B70" t="inlineStr">
         <is>
           <t>11:20</t>
         </is>
       </c>
+      <c r="C70" t="n">
+        <v>267</v>
+      </c>
       <c r="D70" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E70" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F70" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B71" t="n">
-        <v>690</v>
-      </c>
-      <c r="C71" t="inlineStr">
+      <c r="B71" t="inlineStr">
         <is>
           <t>11:30</t>
         </is>
       </c>
+      <c r="C71" t="n">
+        <v>267</v>
+      </c>
       <c r="D71" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E71" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F71" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B72" t="n">
-        <v>700</v>
-      </c>
-      <c r="C72" t="inlineStr">
+      <c r="B72" t="inlineStr">
         <is>
           <t>11:40</t>
         </is>
       </c>
+      <c r="C72" t="n">
+        <v>267</v>
+      </c>
       <c r="D72" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E72" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F72" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B73" t="n">
-        <v>710</v>
-      </c>
-      <c r="C73" t="inlineStr">
+      <c r="B73" t="inlineStr">
         <is>
           <t>11:50</t>
         </is>
       </c>
+      <c r="C73" t="n">
+        <v>267</v>
+      </c>
       <c r="D73" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E73" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F73" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B74" t="n">
-        <v>720</v>
-      </c>
-      <c r="C74" t="inlineStr">
+      <c r="B74" t="inlineStr">
         <is>
           <t>12:00</t>
         </is>
       </c>
+      <c r="C74" t="n">
+        <v>267</v>
+      </c>
       <c r="D74" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E74" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F74" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B75" t="n">
-        <v>730</v>
-      </c>
-      <c r="C75" t="inlineStr">
+      <c r="B75" t="inlineStr">
         <is>
           <t>12:10</t>
         </is>
       </c>
+      <c r="C75" t="n">
+        <v>267</v>
+      </c>
       <c r="D75" t="n">
-        <v>118.272</v>
+        <v>119.616</v>
       </c>
       <c r="E75" t="n">
-        <v>148.736</v>
+        <v>347</v>
+      </c>
+      <c r="F75" t="n">
+        <v>155.456</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B76" t="n">
-        <v>740</v>
-      </c>
-      <c r="C76" t="inlineStr">
+      <c r="B76" t="inlineStr">
         <is>
           <t>12:20</t>
         </is>
       </c>
+      <c r="C76" t="n">
+        <v>267</v>
+      </c>
       <c r="D76" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E76" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F76" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B77" t="n">
-        <v>750</v>
-      </c>
-      <c r="C77" t="inlineStr">
+      <c r="B77" t="inlineStr">
         <is>
           <t>12:30</t>
         </is>
       </c>
+      <c r="C77" t="n">
+        <v>267</v>
+      </c>
       <c r="D77" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E77" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F77" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B78" t="n">
-        <v>760</v>
-      </c>
-      <c r="C78" t="inlineStr">
+      <c r="B78" t="inlineStr">
         <is>
           <t>12:40</t>
         </is>
       </c>
+      <c r="C78" t="n">
+        <v>267</v>
+      </c>
       <c r="D78" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E78" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F78" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B79" t="n">
-        <v>770</v>
-      </c>
-      <c r="C79" t="inlineStr">
+      <c r="B79" t="inlineStr">
         <is>
           <t>12:50</t>
         </is>
       </c>
+      <c r="C79" t="n">
+        <v>267</v>
+      </c>
       <c r="D79" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E79" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F79" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B80" t="n">
-        <v>780</v>
-      </c>
-      <c r="C80" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>13:00</t>
         </is>
       </c>
+      <c r="C80" t="n">
+        <v>267</v>
+      </c>
       <c r="D80" t="n">
-        <v>511.632</v>
+        <v>517.446</v>
       </c>
       <c r="E80" t="n">
-        <v>643.4160000000001</v>
+        <v>347</v>
+      </c>
+      <c r="F80" t="n">
+        <v>672.486</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81" t="n">
-        <v>790</v>
-      </c>
-      <c r="C81" t="inlineStr">
+      <c r="B81" t="inlineStr">
         <is>
           <t>13:10</t>
         </is>
       </c>
+      <c r="C81" t="n">
+        <v>267</v>
+      </c>
       <c r="D81" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E81" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F81" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82" t="n">
-        <v>800</v>
-      </c>
-      <c r="C82" t="inlineStr">
+      <c r="B82" t="inlineStr">
         <is>
           <t>13:20</t>
         </is>
       </c>
+      <c r="C82" t="n">
+        <v>267</v>
+      </c>
       <c r="D82" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E82" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F82" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B83" t="n">
-        <v>810</v>
-      </c>
-      <c r="C83" t="inlineStr">
+      <c r="B83" t="inlineStr">
         <is>
           <t>13:30</t>
         </is>
       </c>
+      <c r="C83" t="n">
+        <v>267</v>
+      </c>
       <c r="D83" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E83" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F83" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84" t="n">
-        <v>820</v>
-      </c>
-      <c r="C84" t="inlineStr">
+      <c r="B84" t="inlineStr">
         <is>
           <t>13:40</t>
         </is>
       </c>
+      <c r="C84" t="n">
+        <v>267</v>
+      </c>
       <c r="D84" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E84" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F84" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85" t="n">
-        <v>830</v>
-      </c>
-      <c r="C85" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>13:50</t>
         </is>
       </c>
+      <c r="C85" t="n">
+        <v>267</v>
+      </c>
       <c r="D85" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E85" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F85" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B86" t="n">
-        <v>840</v>
-      </c>
-      <c r="C86" t="inlineStr">
+      <c r="B86" t="inlineStr">
         <is>
           <t>14:00</t>
         </is>
       </c>
+      <c r="C86" t="n">
+        <v>267</v>
+      </c>
       <c r="D86" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E86" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F86" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="n">
-        <v>850</v>
-      </c>
-      <c r="C87" t="inlineStr">
+      <c r="B87" t="inlineStr">
         <is>
           <t>14:10</t>
         </is>
       </c>
+      <c r="C87" t="n">
+        <v>267</v>
+      </c>
       <c r="D87" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E87" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F87" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B88" t="n">
-        <v>860</v>
-      </c>
-      <c r="C88" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>14:20</t>
         </is>
       </c>
+      <c r="C88" t="n">
+        <v>267</v>
+      </c>
       <c r="D88" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E88" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F88" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B89" t="n">
-        <v>870</v>
-      </c>
-      <c r="C89" t="inlineStr">
+      <c r="B89" t="inlineStr">
         <is>
           <t>14:30</t>
         </is>
       </c>
+      <c r="C89" t="n">
+        <v>267</v>
+      </c>
       <c r="D89" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E89" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F89" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90" t="n">
-        <v>880</v>
-      </c>
-      <c r="C90" t="inlineStr">
+      <c r="B90" t="inlineStr">
         <is>
           <t>14:40</t>
         </is>
       </c>
+      <c r="C90" t="n">
+        <v>267</v>
+      </c>
       <c r="D90" t="n">
-        <v>120.648</v>
+        <v>122.019</v>
       </c>
       <c r="E90" t="n">
-        <v>151.724</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F90" t="n">
+        <v>158.579</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B91" t="n">
-        <v>890</v>
-      </c>
-      <c r="C91" t="inlineStr">
+      <c r="B91" t="inlineStr">
         <is>
           <t>14:50</t>
         </is>
       </c>
+      <c r="C91" t="n">
+        <v>267</v>
+      </c>
       <c r="D91" t="n">
-        <v>120.648</v>
+        <v>122.019</v>
       </c>
       <c r="E91" t="n">
-        <v>151.724</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F91" t="n">
+        <v>158.579</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B92" t="n">
-        <v>900</v>
-      </c>
-      <c r="C92" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t>15:00</t>
         </is>
       </c>
+      <c r="C92" t="n">
+        <v>267</v>
+      </c>
       <c r="D92" t="n">
-        <v>1968.648</v>
+        <v>1991.019</v>
       </c>
       <c r="E92" t="n">
-        <v>2475.724</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F92" t="n">
+        <v>2587.579</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93" t="n">
-        <v>910</v>
-      </c>
-      <c r="C93" t="inlineStr">
+      <c r="B93" t="inlineStr">
         <is>
           <t>15:10</t>
         </is>
       </c>
+      <c r="C93" t="n">
+        <v>267</v>
+      </c>
       <c r="D93" t="n">
-        <v>1995.048</v>
+        <v>2017.719</v>
       </c>
       <c r="E93" t="n">
-        <v>2508.924</v>
+        <v>347</v>
+      </c>
+      <c r="F93" t="n">
+        <v>2622.279</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94" t="n">
-        <v>920</v>
-      </c>
-      <c r="C94" t="inlineStr">
+      <c r="B94" t="inlineStr">
         <is>
           <t>15:20</t>
         </is>
       </c>
+      <c r="C94" t="n">
+        <v>267</v>
+      </c>
       <c r="D94" t="n">
-        <v>1995.048</v>
+        <v>2017.719</v>
       </c>
       <c r="E94" t="n">
-        <v>2508.924</v>
+        <v>347</v>
+      </c>
+      <c r="F94" t="n">
+        <v>2622.279</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B95" t="n">
-        <v>930</v>
-      </c>
-      <c r="C95" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>15:30</t>
         </is>
       </c>
+      <c r="C95" t="n">
+        <v>267</v>
+      </c>
       <c r="D95" t="n">
-        <v>1995.048</v>
+        <v>2017.719</v>
       </c>
       <c r="E95" t="n">
-        <v>2508.924</v>
+        <v>347</v>
+      </c>
+      <c r="F95" t="n">
+        <v>2622.279</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B96" t="n">
-        <v>940</v>
-      </c>
-      <c r="C96" t="inlineStr">
+      <c r="B96" t="inlineStr">
         <is>
           <t>15:40</t>
         </is>
       </c>
+      <c r="C96" t="n">
+        <v>267</v>
+      </c>
       <c r="D96" t="n">
-        <v>1995.048</v>
+        <v>2017.719</v>
       </c>
       <c r="E96" t="n">
-        <v>2508.924</v>
+        <v>347</v>
+      </c>
+      <c r="F96" t="n">
+        <v>2622.279</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B97" t="n">
-        <v>950</v>
-      </c>
-      <c r="C97" t="inlineStr">
+      <c r="B97" t="inlineStr">
         <is>
           <t>15:50</t>
         </is>
       </c>
+      <c r="C97" t="n">
+        <v>267</v>
+      </c>
       <c r="D97" t="n">
-        <v>1995.048</v>
+        <v>2017.719</v>
       </c>
       <c r="E97" t="n">
-        <v>2508.924</v>
+        <v>347</v>
+      </c>
+      <c r="F97" t="n">
+        <v>2622.279</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98" t="n">
-        <v>960</v>
-      </c>
-      <c r="C98" t="inlineStr">
+      <c r="B98" t="inlineStr">
         <is>
           <t>16:00</t>
         </is>
       </c>
+      <c r="C98" t="n">
+        <v>267</v>
+      </c>
       <c r="D98" t="n">
-        <v>326.832</v>
+        <v>330.546</v>
       </c>
       <c r="E98" t="n">
-        <v>411.016</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F98" t="n">
+        <v>429.586</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B99" t="n">
-        <v>970</v>
-      </c>
-      <c r="C99" t="inlineStr">
+      <c r="B99" t="inlineStr">
         <is>
           <t>16:10</t>
         </is>
       </c>
+      <c r="C99" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D99" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E99" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F99" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B100" t="n">
-        <v>980</v>
-      </c>
-      <c r="C100" t="inlineStr">
+      <c r="B100" t="inlineStr">
         <is>
           <t>16:20</t>
         </is>
       </c>
+      <c r="C100" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D100" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E100" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F100" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B101" t="n">
-        <v>990</v>
-      </c>
-      <c r="C101" t="inlineStr">
+      <c r="B101" t="inlineStr">
         <is>
           <t>16:30</t>
         </is>
       </c>
+      <c r="C101" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D101" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E101" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F101" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B102" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C102" t="inlineStr">
+      <c r="B102" t="inlineStr">
         <is>
           <t>16:40</t>
         </is>
       </c>
+      <c r="C102" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D102" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E102" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F102" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B103" t="n">
-        <v>1010</v>
-      </c>
-      <c r="C103" t="inlineStr">
+      <c r="B103" t="inlineStr">
         <is>
           <t>16:50</t>
         </is>
       </c>
+      <c r="C103" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D103" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E103" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F103" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B104" t="n">
-        <v>1020</v>
-      </c>
-      <c r="C104" t="inlineStr">
+      <c r="B104" t="inlineStr">
         <is>
           <t>17:00</t>
         </is>
       </c>
+      <c r="C104" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D104" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E104" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F104" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B105" t="n">
-        <v>1030</v>
-      </c>
-      <c r="C105" t="inlineStr">
+      <c r="B105" t="inlineStr">
         <is>
           <t>17:10</t>
         </is>
       </c>
+      <c r="C105" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D105" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E105" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F105" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B106" t="n">
-        <v>1040</v>
-      </c>
-      <c r="C106" t="inlineStr">
+      <c r="B106" t="inlineStr">
         <is>
           <t>17:20</t>
         </is>
       </c>
+      <c r="C106" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D106" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E106" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F106" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="B107" t="n">
-        <v>1050</v>
-      </c>
-      <c r="C107" t="inlineStr">
+      <c r="B107" t="inlineStr">
         <is>
           <t>17:30</t>
         </is>
       </c>
+      <c r="C107" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D107" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E107" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F107" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="B108" t="n">
-        <v>1060</v>
-      </c>
-      <c r="C108" t="inlineStr">
+      <c r="B108" t="inlineStr">
         <is>
           <t>17:40</t>
         </is>
       </c>
+      <c r="C108" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D108" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E108" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F108" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="B109" t="n">
-        <v>1070</v>
-      </c>
-      <c r="C109" t="inlineStr">
+      <c r="B109" t="inlineStr">
         <is>
           <t>17:50</t>
         </is>
       </c>
+      <c r="C109" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D109" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E109" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F109" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="B110" t="n">
-        <v>1080</v>
-      </c>
-      <c r="C110" t="inlineStr">
+      <c r="B110" t="inlineStr">
         <is>
           <t>18:00</t>
         </is>
       </c>
+      <c r="C110" t="n">
+        <v>267</v>
+      </c>
       <c r="D110" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E110" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F110" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="B111" t="n">
-        <v>1090</v>
-      </c>
-      <c r="C111" t="inlineStr">
+      <c r="B111" t="inlineStr">
         <is>
           <t>18:10</t>
         </is>
       </c>
+      <c r="C111" t="n">
+        <v>267</v>
+      </c>
       <c r="D111" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E111" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F111" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="B112" t="n">
-        <v>1100</v>
-      </c>
-      <c r="C112" t="inlineStr">
+      <c r="B112" t="inlineStr">
         <is>
           <t>18:20</t>
         </is>
       </c>
+      <c r="C112" t="n">
+        <v>267</v>
+      </c>
       <c r="D112" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E112" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F112" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="B113" t="n">
-        <v>1110</v>
-      </c>
-      <c r="C113" t="inlineStr">
+      <c r="B113" t="inlineStr">
         <is>
           <t>18:30</t>
         </is>
       </c>
+      <c r="C113" t="n">
+        <v>267</v>
+      </c>
       <c r="D113" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E113" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F113" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="B114" t="n">
-        <v>1120</v>
-      </c>
-      <c r="C114" t="inlineStr">
+      <c r="B114" t="inlineStr">
         <is>
           <t>18:40</t>
         </is>
       </c>
+      <c r="C114" t="n">
+        <v>267</v>
+      </c>
       <c r="D114" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E114" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F114" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="B115" t="n">
-        <v>1130</v>
-      </c>
-      <c r="C115" t="inlineStr">
+      <c r="B115" t="inlineStr">
         <is>
           <t>18:50</t>
         </is>
       </c>
+      <c r="C115" t="n">
+        <v>267</v>
+      </c>
       <c r="D115" t="n">
-        <v>115.632</v>
+        <v>116.946</v>
       </c>
       <c r="E115" t="n">
-        <v>145.416</v>
+        <v>347</v>
+      </c>
+      <c r="F115" t="n">
+        <v>151.986</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="B116" t="n">
-        <v>1140</v>
-      </c>
-      <c r="C116" t="inlineStr">
+      <c r="B116" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
+      <c r="C116" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D116" t="n">
-        <v>538.032</v>
+        <v>544.146</v>
       </c>
       <c r="E116" t="n">
-        <v>676.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F116" t="n">
+        <v>707.186</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B117" t="n">
-        <v>1150</v>
-      </c>
-      <c r="C117" t="inlineStr">
+      <c r="B117" t="inlineStr">
         <is>
           <t>19:10</t>
         </is>
       </c>
+      <c r="C117" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D117" t="n">
-        <v>142.032</v>
+        <v>143.646</v>
       </c>
       <c r="E117" t="n">
-        <v>178.616</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F117" t="n">
+        <v>186.686</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B118" t="n">
-        <v>1160</v>
-      </c>
-      <c r="C118" t="inlineStr">
+      <c r="B118" t="inlineStr">
         <is>
           <t>19:20</t>
         </is>
       </c>
+      <c r="C118" t="n">
+        <v>267</v>
+      </c>
       <c r="D118" t="n">
-        <v>696.432</v>
+        <v>704.346</v>
       </c>
       <c r="E118" t="n">
-        <v>875.816</v>
+        <v>347</v>
+      </c>
+      <c r="F118" t="n">
+        <v>915.386</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="B119" t="n">
-        <v>1170</v>
-      </c>
-      <c r="C119" t="inlineStr">
+      <c r="B119" t="inlineStr">
         <is>
           <t>19:30</t>
         </is>
       </c>
+      <c r="C119" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D119" t="n">
-        <v>305.712</v>
+        <v>309.186</v>
       </c>
       <c r="E119" t="n">
-        <v>384.456</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F119" t="n">
+        <v>401.826</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="B120" t="n">
-        <v>1180</v>
-      </c>
-      <c r="C120" t="inlineStr">
+      <c r="B120" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
+      <c r="C120" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D120" t="n">
-        <v>305.712</v>
+        <v>309.186</v>
       </c>
       <c r="E120" t="n">
-        <v>384.456</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F120" t="n">
+        <v>401.826</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="B121" t="n">
-        <v>1190</v>
-      </c>
-      <c r="C121" t="inlineStr">
+      <c r="B121" t="inlineStr">
         <is>
           <t>19:50</t>
         </is>
       </c>
+      <c r="C121" t="n">
+        <v>267</v>
+      </c>
       <c r="D121" t="n">
-        <v>332.112</v>
+        <v>335.886</v>
       </c>
       <c r="E121" t="n">
-        <v>417.656</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F121" t="n">
+        <v>436.526</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B122" t="n">
-        <v>1200</v>
-      </c>
-      <c r="C122" t="inlineStr">
+      <c r="B122" t="inlineStr">
         <is>
           <t>20:00</t>
         </is>
       </c>
+      <c r="C122" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D122" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E122" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F122" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="B123" t="n">
-        <v>1210</v>
-      </c>
-      <c r="C123" t="inlineStr">
+      <c r="B123" t="inlineStr">
         <is>
           <t>20:10</t>
         </is>
       </c>
+      <c r="C123" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D123" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E123" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F123" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="B124" t="n">
-        <v>1220</v>
-      </c>
-      <c r="C124" t="inlineStr">
+      <c r="B124" t="inlineStr">
         <is>
           <t>20:20</t>
         </is>
       </c>
+      <c r="C124" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D124" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E124" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F124" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="B125" t="n">
-        <v>1230</v>
-      </c>
-      <c r="C125" t="inlineStr">
+      <c r="B125" t="inlineStr">
         <is>
           <t>20:30</t>
         </is>
       </c>
+      <c r="C125" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D125" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E125" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F125" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="B126" t="n">
-        <v>1240</v>
-      </c>
-      <c r="C126" t="inlineStr">
+      <c r="B126" t="inlineStr">
         <is>
           <t>20:40</t>
         </is>
       </c>
+      <c r="C126" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D126" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E126" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F126" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="B127" t="n">
-        <v>1250</v>
-      </c>
-      <c r="C127" t="inlineStr">
+      <c r="B127" t="inlineStr">
         <is>
           <t>20:50</t>
         </is>
       </c>
+      <c r="C127" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D127" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E127" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F127" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="B128" t="n">
-        <v>1260</v>
-      </c>
-      <c r="C128" t="inlineStr">
+      <c r="B128" t="inlineStr">
         <is>
           <t>21:00</t>
         </is>
       </c>
+      <c r="C128" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D128" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E128" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F128" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="B129" t="n">
-        <v>1270</v>
-      </c>
-      <c r="C129" t="inlineStr">
+      <c r="B129" t="inlineStr">
         <is>
           <t>21:10</t>
         </is>
       </c>
+      <c r="C129" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D129" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E129" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F129" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="B130" t="n">
-        <v>1280</v>
-      </c>
-      <c r="C130" t="inlineStr">
+      <c r="B130" t="inlineStr">
         <is>
           <t>21:20</t>
         </is>
       </c>
+      <c r="C130" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D130" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E130" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F130" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="B131" t="n">
-        <v>1290</v>
-      </c>
-      <c r="C131" t="inlineStr">
+      <c r="B131" t="inlineStr">
         <is>
           <t>21:30</t>
         </is>
       </c>
+      <c r="C131" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D131" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E131" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F131" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="B132" t="n">
-        <v>1300</v>
-      </c>
-      <c r="C132" t="inlineStr">
+      <c r="B132" t="inlineStr">
         <is>
           <t>21:40</t>
         </is>
       </c>
+      <c r="C132" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D132" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E132" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F132" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="B133" t="n">
-        <v>1310</v>
-      </c>
-      <c r="C133" t="inlineStr">
+      <c r="B133" t="inlineStr">
         <is>
           <t>21:50</t>
         </is>
       </c>
+      <c r="C133" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D133" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E133" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F133" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="B134" t="n">
-        <v>1320</v>
-      </c>
-      <c r="C134" t="inlineStr">
+      <c r="B134" t="inlineStr">
         <is>
           <t>22:00</t>
         </is>
       </c>
+      <c r="C134" t="n">
+        <v>267</v>
+      </c>
       <c r="D134" t="n">
-        <v>543.312</v>
+        <v>549.486</v>
       </c>
       <c r="E134" t="n">
-        <v>683.256</v>
+        <v>347</v>
+      </c>
+      <c r="F134" t="n">
+        <v>714.126</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="B135" t="n">
-        <v>1330</v>
-      </c>
-      <c r="C135" t="inlineStr">
+      <c r="B135" t="inlineStr">
         <is>
           <t>22:10</t>
         </is>
       </c>
+      <c r="C135" t="n">
+        <v>266.9999999999999</v>
+      </c>
       <c r="D135" t="n">
-        <v>147.312</v>
+        <v>148.986</v>
       </c>
       <c r="E135" t="n">
-        <v>185.256</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F135" t="n">
+        <v>193.626</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="B136" t="n">
-        <v>1340</v>
-      </c>
-      <c r="C136" t="inlineStr">
+      <c r="B136" t="inlineStr">
         <is>
           <t>22:20</t>
         </is>
       </c>
+      <c r="C136" t="n">
+        <v>267</v>
+      </c>
       <c r="D136" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E136" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F136" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="B137" t="n">
-        <v>1350</v>
-      </c>
-      <c r="C137" t="inlineStr">
+      <c r="B137" t="inlineStr">
         <is>
           <t>22:30</t>
         </is>
       </c>
+      <c r="C137" t="n">
+        <v>267</v>
+      </c>
       <c r="D137" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E137" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F137" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="B138" t="n">
-        <v>1360</v>
-      </c>
-      <c r="C138" t="inlineStr">
+      <c r="B138" t="inlineStr">
         <is>
           <t>22:40</t>
         </is>
       </c>
+      <c r="C138" t="n">
+        <v>267</v>
+      </c>
       <c r="D138" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E138" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F138" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="B139" t="n">
-        <v>1370</v>
-      </c>
-      <c r="C139" t="inlineStr">
+      <c r="B139" t="inlineStr">
         <is>
           <t>22:50</t>
         </is>
       </c>
+      <c r="C139" t="n">
+        <v>267</v>
+      </c>
       <c r="D139" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E139" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F139" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="B140" t="n">
-        <v>1380</v>
-      </c>
-      <c r="C140" t="inlineStr">
+      <c r="B140" t="inlineStr">
         <is>
           <t>23:00</t>
         </is>
       </c>
+      <c r="C140" t="n">
+        <v>267</v>
+      </c>
       <c r="D140" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E140" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F140" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="B141" t="n">
-        <v>1390</v>
-      </c>
-      <c r="C141" t="inlineStr">
+      <c r="B141" t="inlineStr">
         <is>
           <t>23:10</t>
         </is>
       </c>
+      <c r="C141" t="n">
+        <v>267</v>
+      </c>
       <c r="D141" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E141" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F141" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="B142" t="n">
-        <v>1400</v>
-      </c>
-      <c r="C142" t="inlineStr">
+      <c r="B142" t="inlineStr">
         <is>
           <t>23:20</t>
         </is>
       </c>
+      <c r="C142" t="n">
+        <v>267</v>
+      </c>
       <c r="D142" t="n">
-        <v>466.752</v>
+        <v>472.056</v>
       </c>
       <c r="E142" t="n">
-        <v>586.976</v>
+        <v>347</v>
+      </c>
+      <c r="F142" t="n">
+        <v>613.496</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="B143" t="n">
-        <v>1410</v>
-      </c>
-      <c r="C143" t="inlineStr">
+      <c r="B143" t="inlineStr">
         <is>
           <t>23:30</t>
         </is>
       </c>
+      <c r="C143" t="n">
+        <v>267</v>
+      </c>
       <c r="D143" t="n">
-        <v>466.752</v>
+        <v>472.056</v>
       </c>
       <c r="E143" t="n">
-        <v>586.976</v>
+        <v>347</v>
+      </c>
+      <c r="F143" t="n">
+        <v>613.496</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="B144" t="n">
-        <v>1420</v>
-      </c>
-      <c r="C144" t="inlineStr">
+      <c r="B144" t="inlineStr">
         <is>
           <t>23:40</t>
         </is>
       </c>
+      <c r="C144" t="n">
+        <v>267</v>
+      </c>
       <c r="D144" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E144" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F144" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="B145" t="n">
-        <v>1430</v>
-      </c>
-      <c r="C145" t="inlineStr">
+      <c r="B145" t="inlineStr">
         <is>
           <t>23:50</t>
         </is>
       </c>
+      <c r="C145" t="n">
+        <v>267</v>
+      </c>
       <c r="D145" t="n">
-        <v>149.952</v>
+        <v>151.656</v>
       </c>
       <c r="E145" t="n">
-        <v>188.576</v>
+        <v>347.0000000000001</v>
+      </c>
+      <c r="F145" t="n">
+        <v>197.096</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="B146" t="n">
-        <v>1440</v>
-      </c>
-      <c r="C146" t="inlineStr">
+      <c r="B146" t="inlineStr">
         <is>
           <t>00:00</t>
         </is>
       </c>
+      <c r="C146" t="inlineStr"/>
       <c r="D146" t="n">
         <v>0</v>
       </c>
-      <c r="E146" t="n">
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>